<commit_message>
test resource files updates/fixes
</commit_message>
<xml_diff>
--- a/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile4.xlsx
+++ b/enmexcelparser/src/test/resources/net/enanomapper/parser/testExcelParser/testfile4.xlsx
@@ -5,17 +5,17 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\nmdataparser\enmexcelparser\src\test\resources\net\enanomapper\parser\testExcelParser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git-repositories\nmdataparser\enmexcelparser\src\test\resources\net\enanomapper\parser\testExcelParser\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="2960" windowWidth="31860" windowHeight="15060" activeTab="1"/>
+    <workbookView xWindow="2040" yWindow="2955" windowWidth="31860" windowHeight="15060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test conditions" sheetId="4" r:id="rId1"/>
     <sheet name="Test results" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="18">
   <si>
     <t>Time points (hours - or specify any other units):</t>
   </si>
   <si>
     <t>T1</t>
-  </si>
-  <si>
-    <t>T2</t>
   </si>
   <si>
     <t>Alter or add as necessary</t>
@@ -87,7 +84,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -558,15 +555,15 @@
   <dimension ref="A1:AO10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.1796875" customWidth="1"/>
+    <col min="1" max="1" width="44.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -607,50 +604,50 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
       <c r="AE2" s="5"/>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="AE3" s="5"/>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="AE4" s="5"/>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="C5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="D5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="E5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="F5" s="12" t="s">
         <v>8</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>9</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="13">
         <v>0</v>
@@ -671,7 +668,7 @@
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>0</v>
       </c>
@@ -681,9 +678,9 @@
       <c r="C8" s="9"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" s="11">
         <v>6</v>
@@ -695,7 +692,7 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
     </row>
   </sheetData>
@@ -713,70 +710,70 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="16.08984375" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" customWidth="1"/>
-    <col min="8" max="8" width="11.54296875" customWidth="1"/>
-    <col min="9" max="9" width="14.54296875" customWidth="1"/>
-    <col min="14" max="14" width="14.6328125" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>0</v>
       </c>
@@ -805,7 +802,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="D6">
         <v>1</v>
@@ -835,7 +832,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>5</v>
       </c>
@@ -864,7 +861,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>10</v>
       </c>
@@ -893,7 +890,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>25</v>
       </c>
@@ -922,73 +919,73 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10">
         <v>0.91</v>
       </c>
       <c r="I10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J10">
         <v>0.92</v>
       </c>
       <c r="N10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O10">
         <v>0.93</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M12" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>0</v>
       </c>
@@ -1017,7 +1014,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D15">
         <v>1</v>
       </c>
@@ -1046,7 +1043,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D16">
         <v>5</v>
       </c>
@@ -1075,7 +1072,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="4:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D17">
         <v>10</v>
       </c>
@@ -1104,7 +1101,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="4:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D18">
         <v>25</v>
       </c>
@@ -1133,21 +1130,21 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="4:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E19">
         <v>0.91200000000000003</v>
       </c>
       <c r="I19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J19">
         <v>0.92200000000000004</v>
       </c>
       <c r="N19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O19">
         <v>0.93200000000000005</v>

</xml_diff>